<commit_message>
Adicionado alertas e logs do maestro
</commit_message>
<xml_diff>
--- a/resources/moedas_atualizadas.xlsx
+++ b/resources/moedas_atualizadas.xlsx
@@ -486,12 +486,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>5,56</t>
+          <t>5,57</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>10 de jun., 17:13 UTC ·</t>
+          <t>11 de jun., 12:13 UTC ·</t>
         </is>
       </c>
     </row>
@@ -516,12 +516,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>6,35</t>
+          <t>6,37</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>10 de jun., 17:13 UTC ·</t>
+          <t>11 de jun., 12:13 UTC ·</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>10 de jun., 17:13 UTC ·</t>
+          <t>11 de jun., 12:13 UTC ·</t>
         </is>
       </c>
     </row>
@@ -576,12 +576,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>7,51</t>
+          <t>7,52</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>10 de jun., 17:12 UTC ·</t>
+          <t>11 de jun., 12:13 UTC ·</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>10 de jun., 17:12 UTC ·</t>
+          <t>11 de jun., 12:13 UTC ·</t>
         </is>
       </c>
     </row>
@@ -636,12 +636,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>6,76</t>
+          <t>6,77</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>10 de jun., 17:13 UTC ·</t>
+          <t>11 de jun., 12:13 UTC ·</t>
         </is>
       </c>
     </row>
@@ -666,12 +666,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>3,63</t>
+          <t>3,62</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>10 de jun., 17:11 UTC ·</t>
+          <t>11 de jun., 12:13 UTC ·</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>10 de jun., 17:11 UTC ·</t>
+          <t>11 de jun., 12:13 UTC ·</t>
         </is>
       </c>
     </row>
@@ -731,7 +731,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>10 de jun., 17:13 UTC ·</t>
+          <t>11 de jun., 12:12 UTC ·</t>
         </is>
       </c>
     </row>
@@ -761,7 +761,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>10 de jun., 17:13 UTC ·</t>
+          <t>11 de jun., 12:13 UTC ·</t>
         </is>
       </c>
     </row>
@@ -786,12 +786,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0,77</t>
+          <t>0,78</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>10 de jun., 17:13 UTC ·</t>
+          <t>11 de jun., 12:14 UTC ·</t>
         </is>
       </c>
     </row>
@@ -821,7 +821,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>10 de jun., 17:12 UTC ·</t>
+          <t>11 de jun., 12:12 UTC ·</t>
         </is>
       </c>
     </row>
@@ -851,7 +851,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>10 de jun., 11:19 UTC ·</t>
+          <t>11 de jun., 11:19 UTC ·</t>
         </is>
       </c>
     </row>
@@ -881,7 +881,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>10 de jun., 17:13 UTC ·</t>
+          <t>11 de jun., 12:09 UTC ·</t>
         </is>
       </c>
     </row>
@@ -911,7 +911,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>10 de jun., 17:13 UTC ·</t>
+          <t>11 de jun., 12:13 UTC ·</t>
         </is>
       </c>
     </row>
@@ -936,12 +936,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1,09</t>
+          <t>1,07</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>10 de jun., 17:11 UTC ·</t>
+          <t>11 de jun., 12:13 UTC ·</t>
         </is>
       </c>
     </row>
@@ -971,7 +971,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>10 de jun., 17:12 UTC ·</t>
+          <t>11 de jun., 12:13 UTC ·</t>
         </is>
       </c>
     </row>
@@ -996,12 +996,12 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>4,32</t>
+          <t>4,33</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>10 de jun., 17:11 UTC ·</t>
+          <t>11 de jun., 12:13 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>10 de jun., 17:12 UTC ·</t>
+          <t>11 de jun., 12:13 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1056,12 +1056,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>4,17</t>
+          <t>4,16</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>10 de jun., 17:12 UTC ·</t>
+          <t>11 de jun., 12:13 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>10 de jun., 17:12 UTC ·</t>
+          <t>11 de jun., 12:13 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1116,12 +1116,12 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>3,49</t>
+          <t>3,50</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>10 de jun., 17:12 UTC ·</t>
+          <t>11 de jun., 12:13 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1146,12 +1146,12 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0,77</t>
+          <t>0,78</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>10 de jun., 17:13 UTC ·</t>
+          <t>11 de jun., 12:14 UTC ·</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Melhoria na estruturação do projeto
</commit_message>
<xml_diff>
--- a/resources/moedas_atualizadas.xlsx
+++ b/resources/moedas_atualizadas.xlsx
@@ -491,7 +491,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>11 de jun., 13:18 UTC ·</t>
+          <t>11 de jun., 13:52 UTC ·</t>
         </is>
       </c>
     </row>
@@ -521,7 +521,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>11 de jun., 13:16 UTC ·</t>
+          <t>11 de jun., 13:53 UTC ·</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>11 de jun., 13:18 UTC ·</t>
+          <t>11 de jun., 13:53 UTC ·</t>
         </is>
       </c>
     </row>
@@ -576,12 +576,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>7,51</t>
+          <t>7,50</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>11 de jun., 13:19 UTC ·</t>
+          <t>11 de jun., 13:52 UTC ·</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>11 de jun., 13:19 UTC ·</t>
+          <t>11 de jun., 13:52 UTC ·</t>
         </is>
       </c>
     </row>
@@ -641,7 +641,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>11 de jun., 13:19 UTC ·</t>
+          <t>11 de jun., 13:53 UTC ·</t>
         </is>
       </c>
     </row>
@@ -671,7 +671,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>11 de jun., 13:19 UTC ·</t>
+          <t>11 de jun., 13:51 UTC ·</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>11 de jun., 13:19 UTC ·</t>
+          <t>11 de jun., 13:53 UTC ·</t>
         </is>
       </c>
     </row>
@@ -731,7 +731,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>11 de jun., 13:16 UTC ·</t>
+          <t>11 de jun., 13:53 UTC ·</t>
         </is>
       </c>
     </row>
@@ -761,7 +761,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>11 de jun., 13:19 UTC ·</t>
+          <t>11 de jun., 13:53 UTC ·</t>
         </is>
       </c>
     </row>
@@ -791,7 +791,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>11 de jun., 13:19 UTC ·</t>
+          <t>11 de jun., 13:53 UTC ·</t>
         </is>
       </c>
     </row>
@@ -821,7 +821,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>11 de jun., 13:18 UTC ·</t>
+          <t>11 de jun., 13:52 UTC ·</t>
         </is>
       </c>
     </row>
@@ -881,7 +881,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>11 de jun., 13:19 UTC ·</t>
+          <t>11 de jun., 13:52 UTC ·</t>
         </is>
       </c>
     </row>
@@ -911,7 +911,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>11 de jun., 13:16 UTC ·</t>
+          <t>11 de jun., 13:53 UTC ·</t>
         </is>
       </c>
     </row>
@@ -941,7 +941,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>11 de jun., 13:18 UTC ·</t>
+          <t>11 de jun., 13:52 UTC ·</t>
         </is>
       </c>
     </row>
@@ -971,7 +971,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>11 de jun., 13:18 UTC ·</t>
+          <t>11 de jun., 13:52 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>11 de jun., 13:16 UTC ·</t>
+          <t>11 de jun., 13:53 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>11 de jun., 13:18 UTC ·</t>
+          <t>11 de jun., 13:52 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>11 de jun., 13:19 UTC ·</t>
+          <t>11 de jun., 13:53 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>11 de jun., 13:18 UTC ·</t>
+          <t>11 de jun., 13:52 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1121,7 +1121,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>11 de jun., 13:18 UTC ·</t>
+          <t>11 de jun., 13:53 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>11 de jun., 13:19 UTC ·</t>
+          <t>11 de jun., 13:53 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>11 de jun., 13:19 UTC ·</t>
+          <t>11 de jun., 13:53 UTC ·</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Tests adicionados e update no readme
</commit_message>
<xml_diff>
--- a/resources/moedas_atualizadas.xlsx
+++ b/resources/moedas_atualizadas.xlsx
@@ -486,12 +486,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>5,55</t>
+          <t>5,53</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>11 de jun., 13:52 UTC ·</t>
+          <t>11 de jun., 16:37 UTC ·</t>
         </is>
       </c>
     </row>
@@ -516,12 +516,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>6,37</t>
+          <t>6,36</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>11 de jun., 13:53 UTC ·</t>
+          <t>11 de jun., 16:36 UTC ·</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>11 de jun., 13:53 UTC ·</t>
+          <t>11 de jun., 16:37 UTC ·</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>11 de jun., 13:52 UTC ·</t>
+          <t>11 de jun., 16:37 UTC ·</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>11 de jun., 13:52 UTC ·</t>
+          <t>11 de jun., 16:37 UTC ·</t>
         </is>
       </c>
     </row>
@@ -636,12 +636,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>6,77</t>
+          <t>6,75</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>11 de jun., 13:53 UTC ·</t>
+          <t>11 de jun., 16:36 UTC ·</t>
         </is>
       </c>
     </row>
@@ -666,12 +666,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>3,62</t>
+          <t>3,61</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>11 de jun., 13:51 UTC ·</t>
+          <t>11 de jun., 16:36 UTC ·</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>11 de jun., 13:53 UTC ·</t>
+          <t>11 de jun., 16:36 UTC ·</t>
         </is>
       </c>
     </row>
@@ -726,12 +726,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>4,06</t>
+          <t>4,05</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>11 de jun., 13:53 UTC ·</t>
+          <t>11 de jun., 16:36 UTC ·</t>
         </is>
       </c>
     </row>
@@ -761,7 +761,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>11 de jun., 13:53 UTC ·</t>
+          <t>11 de jun., 16:36 UTC ·</t>
         </is>
       </c>
     </row>
@@ -791,7 +791,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>11 de jun., 13:53 UTC ·</t>
+          <t>11 de jun., 16:37 UTC ·</t>
         </is>
       </c>
     </row>
@@ -821,7 +821,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>11 de jun., 13:52 UTC ·</t>
+          <t>11 de jun., 16:37 UTC ·</t>
         </is>
       </c>
     </row>
@@ -881,7 +881,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>11 de jun., 13:52 UTC ·</t>
+          <t>11 de jun., 16:36 UTC ·</t>
         </is>
       </c>
     </row>
@@ -911,7 +911,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>11 de jun., 13:53 UTC ·</t>
+          <t>11 de jun., 16:36 UTC ·</t>
         </is>
       </c>
     </row>
@@ -941,7 +941,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>11 de jun., 13:52 UTC ·</t>
+          <t>11 de jun., 16:37 UTC ·</t>
         </is>
       </c>
     </row>
@@ -971,7 +971,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>11 de jun., 13:52 UTC ·</t>
+          <t>11 de jun., 16:37 UTC ·</t>
         </is>
       </c>
     </row>
@@ -996,12 +996,12 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>4,32</t>
+          <t>4,31</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>11 de jun., 13:53 UTC ·</t>
+          <t>11 de jun., 16:36 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>11 de jun., 13:52 UTC ·</t>
+          <t>11 de jun., 16:37 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1056,12 +1056,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>4,16</t>
+          <t>4,15</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>11 de jun., 13:53 UTC ·</t>
+          <t>11 de jun., 16:37 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>11 de jun., 13:52 UTC ·</t>
+          <t>11 de jun., 16:37 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1121,7 +1121,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>11 de jun., 13:53 UTC ·</t>
+          <t>11 de jun., 16:36 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>11 de jun., 13:53 UTC ·</t>
+          <t>11 de jun., 16:37 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>11 de jun., 13:53 UTC ·</t>
+          <t>11 de jun., 16:37 UTC ·</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Adicionado docker no projeto para poder rodar em container
</commit_message>
<xml_diff>
--- a/resources/moedas_atualizadas.xlsx
+++ b/resources/moedas_atualizadas.xlsx
@@ -486,12 +486,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>5,53</t>
+          <t>5,54</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>11 de jun., 16:37 UTC ·</t>
+          <t>11 de jun., 18:46 UTC ·</t>
         </is>
       </c>
     </row>
@@ -516,12 +516,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>6,36</t>
+          <t>6,37</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>11 de jun., 16:36 UTC ·</t>
+          <t>11 de jun., 18:46 UTC ·</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>11 de jun., 16:37 UTC ·</t>
+          <t>11 de jun., 18:46 UTC ·</t>
         </is>
       </c>
     </row>
@@ -576,12 +576,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>7,50</t>
+          <t>7,51</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>11 de jun., 16:37 UTC ·</t>
+          <t>11 de jun., 18:46 UTC ·</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>11 de jun., 16:37 UTC ·</t>
+          <t>11 de jun., 18:47 UTC ·</t>
         </is>
       </c>
     </row>
@@ -641,7 +641,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>11 de jun., 16:36 UTC ·</t>
+          <t>11 de jun., 18:46 UTC ·</t>
         </is>
       </c>
     </row>
@@ -671,7 +671,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>11 de jun., 16:36 UTC ·</t>
+          <t>11 de jun., 18:46 UTC ·</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>11 de jun., 16:36 UTC ·</t>
+          <t>11 de jun., 18:46 UTC ·</t>
         </is>
       </c>
     </row>
@@ -726,12 +726,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>4,05</t>
+          <t>4,06</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>11 de jun., 16:36 UTC ·</t>
+          <t>11 de jun., 18:46 UTC ·</t>
         </is>
       </c>
     </row>
@@ -761,7 +761,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>11 de jun., 16:36 UTC ·</t>
+          <t>11 de jun., 18:46 UTC ·</t>
         </is>
       </c>
     </row>
@@ -791,7 +791,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>11 de jun., 16:37 UTC ·</t>
+          <t>11 de jun., 18:45 UTC ·</t>
         </is>
       </c>
     </row>
@@ -821,7 +821,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>11 de jun., 16:37 UTC ·</t>
+          <t>11 de jun., 18:45 UTC ·</t>
         </is>
       </c>
     </row>
@@ -881,7 +881,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>11 de jun., 16:36 UTC ·</t>
+          <t>11 de jun., 18:46 UTC ·</t>
         </is>
       </c>
     </row>
@@ -911,7 +911,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>11 de jun., 16:36 UTC ·</t>
+          <t>11 de jun., 18:46 UTC ·</t>
         </is>
       </c>
     </row>
@@ -941,7 +941,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>11 de jun., 16:37 UTC ·</t>
+          <t>11 de jun., 18:46 UTC ·</t>
         </is>
       </c>
     </row>
@@ -971,7 +971,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>11 de jun., 16:37 UTC ·</t>
+          <t>11 de jun., 18:46 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>11 de jun., 16:36 UTC ·</t>
+          <t>11 de jun., 18:46 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>11 de jun., 16:37 UTC ·</t>
+          <t>11 de jun., 18:46 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1056,12 +1056,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>4,15</t>
+          <t>4,16</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>11 de jun., 16:37 UTC ·</t>
+          <t>11 de jun., 18:47 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>11 de jun., 16:37 UTC ·</t>
+          <t>11 de jun., 18:46 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1121,7 +1121,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>11 de jun., 16:36 UTC ·</t>
+          <t>11 de jun., 18:45 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>11 de jun., 16:37 UTC ·</t>
+          <t>11 de jun., 18:45 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>11 de jun., 16:37 UTC ·</t>
+          <t>11 de jun., 18:47 UTC ·</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Projeto atualizado com algumas melhorias de codigo
</commit_message>
<xml_diff>
--- a/resources/moedas_atualizadas.xlsx
+++ b/resources/moedas_atualizadas.xlsx
@@ -486,12 +486,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>5,54</t>
+          <t>5,49</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>11 de jun., 18:46 UTC ·</t>
+          <t>16 de jun., 19:31 UTC ·</t>
         </is>
       </c>
     </row>
@@ -516,12 +516,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>6,37</t>
+          <t>6,36</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>11 de jun., 18:46 UTC ·</t>
+          <t>16 de jun., 19:26 UTC ·</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>11 de jun., 18:46 UTC ·</t>
+          <t>16 de jun., 19:31 UTC ·</t>
         </is>
       </c>
     </row>
@@ -576,12 +576,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>7,51</t>
+          <t>7,47</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>11 de jun., 18:46 UTC ·</t>
+          <t>16 de jun., 19:30 UTC ·</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>11 de jun., 18:47 UTC ·</t>
+          <t>16 de jun., 19:30 UTC ·</t>
         </is>
       </c>
     </row>
@@ -641,7 +641,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>11 de jun., 18:46 UTC ·</t>
+          <t>16 de jun., 19:26 UTC ·</t>
         </is>
       </c>
     </row>
@@ -666,12 +666,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>3,61</t>
+          <t>3,59</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>11 de jun., 18:46 UTC ·</t>
+          <t>16 de jun., 19:31 UTC ·</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>11 de jun., 18:46 UTC ·</t>
+          <t>16 de jun., 19:31 UTC ·</t>
         </is>
       </c>
     </row>
@@ -726,12 +726,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>4,06</t>
+          <t>4,05</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>11 de jun., 18:46 UTC ·</t>
+          <t>16 de jun., 19:31 UTC ·</t>
         </is>
       </c>
     </row>
@@ -756,12 +756,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0,71</t>
+          <t>0,70</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>11 de jun., 18:46 UTC ·</t>
+          <t>16 de jun., 19:31 UTC ·</t>
         </is>
       </c>
     </row>
@@ -791,7 +791,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>11 de jun., 18:45 UTC ·</t>
+          <t>16 de jun., 19:29 UTC ·</t>
         </is>
       </c>
     </row>
@@ -816,12 +816,12 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0,065</t>
+          <t>0,064</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>11 de jun., 18:45 UTC ·</t>
+          <t>16 de jun., 19:30 UTC ·</t>
         </is>
       </c>
     </row>
@@ -851,7 +851,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>11 de jun., 11:19 UTC ·</t>
+          <t>16 de jun., 11:19 UTC ·</t>
         </is>
       </c>
     </row>
@@ -876,12 +876,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0,0047</t>
+          <t>0,0046</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>11 de jun., 18:46 UTC ·</t>
+          <t>16 de jun., 19:30 UTC ·</t>
         </is>
       </c>
     </row>
@@ -911,7 +911,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>11 de jun., 18:46 UTC ·</t>
+          <t>16 de jun., 19:31 UTC ·</t>
         </is>
       </c>
     </row>
@@ -936,12 +936,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1,08</t>
+          <t>1,09</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>11 de jun., 18:46 UTC ·</t>
+          <t>16 de jun., 19:30 UTC ·</t>
         </is>
       </c>
     </row>
@@ -966,12 +966,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1,48</t>
+          <t>1,46</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>11 de jun., 18:46 UTC ·</t>
+          <t>16 de jun., 19:30 UTC ·</t>
         </is>
       </c>
     </row>
@@ -996,12 +996,12 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>4,31</t>
+          <t>4,29</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>11 de jun., 18:46 UTC ·</t>
+          <t>16 de jun., 19:31 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1026,12 +1026,12 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0,099</t>
+          <t>0,097</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>11 de jun., 18:46 UTC ·</t>
+          <t>16 de jun., 19:30 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1056,12 +1056,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>4,16</t>
+          <t>4,11</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>11 de jun., 18:47 UTC ·</t>
+          <t>16 de jun., 19:31 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>11 de jun., 18:46 UTC ·</t>
+          <t>16 de jun., 19:30 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1121,7 +1121,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>11 de jun., 18:45 UTC ·</t>
+          <t>16 de jun., 19:29 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>11 de jun., 18:45 UTC ·</t>
+          <t>16 de jun., 19:29 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>11 de jun., 18:47 UTC ·</t>
+          <t>16 de jun., 19:31 UTC ·</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Melhoria nas nomenclaturas de arquivos e de classes
</commit_message>
<xml_diff>
--- a/resources/moedas_atualizadas.xlsx
+++ b/resources/moedas_atualizadas.xlsx
@@ -486,12 +486,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>5,49</t>
+          <t>5,50</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>16 de jun., 19:31 UTC ·</t>
+          <t>17 de jun., 18:34 UTC ·</t>
         </is>
       </c>
     </row>
@@ -516,12 +516,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>6,36</t>
+          <t>6,32</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>16 de jun., 19:26 UTC ·</t>
+          <t>17 de jun., 18:33 UTC ·</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>16 de jun., 19:31 UTC ·</t>
+          <t>17 de jun., 18:34 UTC ·</t>
         </is>
       </c>
     </row>
@@ -576,12 +576,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>7,47</t>
+          <t>7,39</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>16 de jun., 19:30 UTC ·</t>
+          <t>17 de jun., 18:32 UTC ·</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>16 de jun., 19:30 UTC ·</t>
+          <t>17 de jun., 18:34 UTC ·</t>
         </is>
       </c>
     </row>
@@ -636,12 +636,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>6,75</t>
+          <t>6,74</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>16 de jun., 19:26 UTC ·</t>
+          <t>17 de jun., 18:33 UTC ·</t>
         </is>
       </c>
     </row>
@@ -666,12 +666,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>3,59</t>
+          <t>3,56</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>16 de jun., 19:31 UTC ·</t>
+          <t>17 de jun., 18:33 UTC ·</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>16 de jun., 19:31 UTC ·</t>
+          <t>17 de jun., 18:33 UTC ·</t>
         </is>
       </c>
     </row>
@@ -726,12 +726,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>4,05</t>
+          <t>4,03</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>16 de jun., 19:31 UTC ·</t>
+          <t>17 de jun., 18:33 UTC ·</t>
         </is>
       </c>
     </row>
@@ -761,7 +761,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>16 de jun., 19:31 UTC ·</t>
+          <t>17 de jun., 18:33 UTC ·</t>
         </is>
       </c>
     </row>
@@ -791,7 +791,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>16 de jun., 19:29 UTC ·</t>
+          <t>17 de jun., 18:34 UTC ·</t>
         </is>
       </c>
     </row>
@@ -821,7 +821,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>16 de jun., 19:30 UTC ·</t>
+          <t>17 de jun., 18:34 UTC ·</t>
         </is>
       </c>
     </row>
@@ -851,7 +851,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>16 de jun., 11:19 UTC ·</t>
+          <t>17 de jun., 11:19 UTC ·</t>
         </is>
       </c>
     </row>
@@ -876,12 +876,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0,0046</t>
+          <t>0,0047</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>16 de jun., 19:30 UTC ·</t>
+          <t>17 de jun., 18:34 UTC ·</t>
         </is>
       </c>
     </row>
@@ -911,7 +911,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>16 de jun., 19:31 UTC ·</t>
+          <t>17 de jun., 18:33 UTC ·</t>
         </is>
       </c>
     </row>
@@ -936,12 +936,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1,09</t>
+          <t>1,10</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>16 de jun., 19:30 UTC ·</t>
+          <t>17 de jun., 18:33 UTC ·</t>
         </is>
       </c>
     </row>
@@ -966,12 +966,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1,46</t>
+          <t>1,47</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>16 de jun., 19:30 UTC ·</t>
+          <t>17 de jun., 18:34 UTC ·</t>
         </is>
       </c>
     </row>
@@ -996,12 +996,12 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>4,29</t>
+          <t>4,28</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>16 de jun., 19:31 UTC ·</t>
+          <t>17 de jun., 18:33 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>16 de jun., 19:30 UTC ·</t>
+          <t>17 de jun., 18:34 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1056,12 +1056,12 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>4,11</t>
+          <t>4,13</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>16 de jun., 19:31 UTC ·</t>
+          <t>17 de jun., 18:34 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>16 de jun., 19:30 UTC ·</t>
+          <t>17 de jun., 18:34 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1116,12 +1116,12 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>3,50</t>
+          <t>3,48</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>16 de jun., 19:29 UTC ·</t>
+          <t>17 de jun., 18:33 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>16 de jun., 19:29 UTC ·</t>
+          <t>17 de jun., 18:34 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>16 de jun., 19:31 UTC ·</t>
+          <t>17 de jun., 18:34 UTC ·</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor bot configuration, enhance README, improve CSV handling, and update tests
</commit_message>
<xml_diff>
--- a/resources/moedas_atualizadas.xlsx
+++ b/resources/moedas_atualizadas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,7 +491,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>17 de jun., 18:34 UTC ·</t>
+          <t>20 de jun., 14:50 UTC ·</t>
         </is>
       </c>
     </row>
@@ -521,7 +521,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>17 de jun., 18:33 UTC ·</t>
+          <t>20 de jun., 14:48 UTC ·</t>
         </is>
       </c>
     </row>
@@ -531,27 +531,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Real</t>
+          <t>Libra Esterlina</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>R$</t>
+          <t>£</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>BRL</t>
+          <t>GBP</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0,18</t>
+          <t>7,40</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>17 de jun., 18:34 UTC ·</t>
+          <t>20 de jun., 14:49 UTC ·</t>
         </is>
       </c>
     </row>
@@ -561,27 +561,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Libra Esterlina</t>
+          <t>Iene</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>£</t>
+          <t>¥</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>GBP</t>
+          <t>JPY</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>7,39</t>
+          <t>0,038</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>17 de jun., 18:32 UTC ·</t>
+          <t>20 de jun., 14:49 UTC ·</t>
         </is>
       </c>
     </row>
@@ -591,27 +591,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Iene</t>
+          <t>Franco Suíço</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>¥</t>
+          <t>CHF</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>JPY</t>
+          <t>CHF</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0,038</t>
+          <t>6,72</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>17 de jun., 18:34 UTC ·</t>
+          <t>20 de jun., 14:48 UTC ·</t>
         </is>
       </c>
     </row>
@@ -621,27 +621,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Franco Suíço</t>
+          <t>Dólar Australiano</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CHF</t>
+          <t>A$</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>CHF</t>
+          <t>AUD</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>6,74</t>
+          <t>3,55</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>17 de jun., 18:33 UTC ·</t>
+          <t>20 de jun., 14:48 UTC ·</t>
         </is>
       </c>
     </row>
@@ -651,27 +651,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Dólar Australiano</t>
+          <t>Peso Mexicano</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>A$</t>
+          <t>$</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>AUD</t>
+          <t>MXN</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>3,56</t>
+          <t>0,29</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>17 de jun., 18:33 UTC ·</t>
+          <t>20 de jun., 14:48 UTC ·</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Peso Mexicano</t>
+          <t>Dólar Canadiano</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -691,17 +691,17 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>MXN</t>
+          <t>CAD</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0,29</t>
+          <t>4,00</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>17 de jun., 18:33 UTC ·</t>
+          <t>20 de jun., 14:48 UTC ·</t>
         </is>
       </c>
     </row>
@@ -711,27 +711,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Dólar Canadiano</t>
+          <t>Dólar de Hong Kong</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>$</t>
+          <t>HK$</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>CAD</t>
+          <t>HKD</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>4,03</t>
+          <t>0,70</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>17 de jun., 18:33 UTC ·</t>
+          <t>20 de jun., 14:48 UTC ·</t>
         </is>
       </c>
     </row>
@@ -741,27 +741,27 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Dólar de Hong Kong</t>
+          <t>Yuan Chinês</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>HK$</t>
+          <t>¥</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>HKD</t>
+          <t>CNY</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0,70</t>
+          <t>0,77</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>17 de jun., 18:33 UTC ·</t>
+          <t>20 de jun., 14:48 UTC ·</t>
         </is>
       </c>
     </row>
@@ -771,27 +771,27 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Yuan Chinês</t>
+          <t>Rúpia Indiana</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>¥</t>
+          <t>₹</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>CNY</t>
+          <t>INR</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0,77</t>
+          <t>0,063</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>17 de jun., 18:34 UTC ·</t>
+          <t>20 de jun., 14:49 UTC ·</t>
         </is>
       </c>
     </row>
@@ -801,27 +801,27 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Rúpia Indiana</t>
+          <t>Peso Chileno</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>₹</t>
+          <t>$</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>INR</t>
+          <t>CLP</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0,064</t>
+          <t>0,0058</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>17 de jun., 18:34 UTC ·</t>
+          <t>20 de jun., 11:19 UTC ·</t>
         </is>
       </c>
     </row>
@@ -831,7 +831,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Peso Chileno</t>
+          <t>Peso Argentino</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -841,17 +841,17 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>CLP</t>
+          <t>ARS</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>0,0059</t>
+          <t>0,0047</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>17 de jun., 11:19 UTC ·</t>
+          <t>20 de jun., 14:48 UTC ·</t>
         </is>
       </c>
     </row>
@@ -861,7 +861,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Peso Argentino</t>
+          <t>Peso Colombiano</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -871,17 +871,17 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>ARS</t>
+          <t>COP</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0,0047</t>
+          <t>0,0013</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>17 de jun., 18:34 UTC ·</t>
+          <t>20 de jun., 14:48 UTC ·</t>
         </is>
       </c>
     </row>
@@ -891,27 +891,27 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Peso Colombiano</t>
+          <t>Rúpia Russa</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>$</t>
+          <t>₽</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>COP</t>
+          <t>RUB</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0,0013</t>
+          <t>1,10</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>17 de jun., 18:33 UTC ·</t>
+          <t>20 de jun., 14:49 UTC ·</t>
         </is>
       </c>
     </row>
@@ -921,27 +921,27 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Rúpia Russa</t>
+          <t>Riyal Saudi</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>₽</t>
+          <t>﷼</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>RUB</t>
+          <t>SAR</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1,10</t>
+          <t>1,46</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>17 de jun., 18:33 UTC ·</t>
+          <t>20 de jun., 14:49 UTC ·</t>
         </is>
       </c>
     </row>
@@ -951,27 +951,27 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Riyal Saudi</t>
+          <t>Dólar de Singapura</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>﷼</t>
+          <t>S$</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>SAR</t>
+          <t>SGD</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1,47</t>
+          <t>4,27</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>17 de jun., 18:34 UTC ·</t>
+          <t>20 de jun., 14:48 UTC ·</t>
         </is>
       </c>
     </row>
@@ -981,27 +981,27 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Dólar de Singapura</t>
+          <t>Peso Filipino</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>S$</t>
+          <t>₱</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>SGD</t>
+          <t>PHP</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>4,28</t>
+          <t>0,096</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>17 de jun., 18:33 UTC ·</t>
+          <t>20 de jun., 14:49 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1011,27 +1011,27 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Peso Filipino</t>
+          <t>Yuan de Taiwan</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>₱</t>
+          <t>NT$</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>PHP</t>
+          <t>TWD</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0,097</t>
+          <t>4,11</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>17 de jun., 18:34 UTC ·</t>
+          <t>20 de jun., 14:50 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1041,27 +1041,27 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Yuan de Taiwan</t>
+          <t>Dinar Iraquiano</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>NT$</t>
+          <t>؋</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>TWD</t>
+          <t>IQD</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>4,13</t>
+          <t>0,0042</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>17 de jun., 18:34 UTC ·</t>
+          <t>20 de jun., 14:49 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1071,27 +1071,27 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Dinar Iraquiano</t>
+          <t>Rúpia Sri Lanka</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>؋</t>
+          <t>Rs</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>IQD</t>
+          <t>LKR</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>0,0042</t>
+          <t>3,47</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>17 de jun., 18:34 UTC ·</t>
+          <t>20 de jun., 14:48 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1101,27 +1101,27 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Rúpia Sri Lanka</t>
+          <t>Yuan Chinês</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Rs</t>
+          <t>¥</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>LKR</t>
+          <t>CNY</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>3,48</t>
+          <t>0,77</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>17 de jun., 18:33 UTC ·</t>
+          <t>20 de jun., 14:48 UTC ·</t>
         </is>
       </c>
     </row>
@@ -1131,57 +1131,27 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Yuan Chinês</t>
+          <t>Won Sul-Coreano</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>¥</t>
+          <t>₩</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>CNY</t>
+          <t>KRW</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0,77</t>
+          <t>0,0040</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>17 de jun., 18:34 UTC ·</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>24</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Won Sul-Coreano</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>₩</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>KRW</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>0,0040</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>17 de jun., 18:34 UTC ·</t>
+          <t>20 de jun., 14:50 UTC ·</t>
         </is>
       </c>
     </row>

</xml_diff>